<commit_message>
feat: execute shell daily
</commit_message>
<xml_diff>
--- a/data/punchTime.xlsx
+++ b/data/punchTime.xlsx
@@ -404,10 +404,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="2" x14ac:dyDescent="0" defaultColWidth="9" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2" x14ac:dyDescent="0" defaultColWidth="9" customHeight="1"/>
   <cols>
     <col min="1" max="3" width="12.625" customWidth="1"/>
   </cols>

</xml_diff>